<commit_message>
last update, company FS inconsistent
</commit_message>
<xml_diff>
--- a/TRUS/TRUS.xlsx
+++ b/TRUS/TRUS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\IDX-DB\TRUS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719EAE65-4A26-4102-8FC1-EFC179187CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F77C96B-A795-4C28-B0BB-A4301BF12B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27930" windowHeight="16440" xr2:uid="{5D664303-5A82-49FF-9278-C015F4931C8B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27690" windowHeight="16200" xr2:uid="{5D664303-5A82-49FF-9278-C015F4931C8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
   <si>
     <t>Q4 2021</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>Q1 2025</t>
-  </si>
-  <si>
-    <t>TV</t>
   </si>
   <si>
     <t>Cash</t>
@@ -307,6 +304,18 @@
   <si>
     <t>Purchase of rented asset</t>
   </si>
+  <si>
+    <t>Q1 2021</t>
+  </si>
+  <si>
+    <t>Q2 2021</t>
+  </si>
+  <si>
+    <t>Q3 2021</t>
+  </si>
+  <si>
+    <t>Investment value loss</t>
+  </si>
 </sst>
 </file>
 
@@ -318,7 +327,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,6 +353,12 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -534,7 +549,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Main!$B$45:$E$45</c:f>
+              <c:f>Main!$E$45:$H$45</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
@@ -600,7 +615,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Main!$B$46:$E$46</c:f>
+              <c:f>Main!$E$46:$H$46</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
@@ -902,7 +917,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Main!$A$56</c:f>
+              <c:f>Main!$A$57</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -935,7 +950,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Main!$B$3:$E$3</c:f>
+              <c:f>Main!$E$3:$H$3</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
@@ -956,7 +971,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Main!$B$56:$E$56</c:f>
+              <c:f>Main!$E$57:$H$57</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2770,254 +2785,306 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7CB97D-BE11-44C8-A0A5-390CF65A0E49}">
-  <dimension ref="A2:R116"/>
+  <dimension ref="A2:U117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68:E68"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="12.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="15" width="13.42578125" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="18" width="8.85546875" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="50" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="19" width="10.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="20" max="21" width="8.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="53" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" s="3">
+        <v>14536</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3">
+        <v>127304</v>
+      </c>
+      <c r="F3" s="3">
+        <v>116424</v>
+      </c>
+      <c r="G3" s="3">
+        <v>86097</v>
+      </c>
+      <c r="H3" s="3">
+        <v>73578</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="3">
-        <v>127304</v>
-      </c>
-      <c r="C3" s="3">
-        <v>116424</v>
-      </c>
-      <c r="D3" s="3">
-        <v>86097</v>
-      </c>
-      <c r="E3" s="3">
-        <v>73578</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" s="3">
+        <v>268623</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3">
+        <v>180513</v>
+      </c>
+      <c r="F4" s="3">
+        <v>197171</v>
+      </c>
+      <c r="G4" s="3">
+        <v>222680</v>
+      </c>
+      <c r="H4" s="3">
+        <v>218831</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="3">
-        <v>180513</v>
-      </c>
-      <c r="C4" s="3">
-        <v>197171</v>
-      </c>
-      <c r="D4" s="3">
-        <v>222680</v>
-      </c>
-      <c r="E4" s="3">
-        <v>218831</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" s="3">
+        <v>22016</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3">
+        <v>29961</v>
+      </c>
+      <c r="F5" s="3">
+        <v>29162</v>
+      </c>
+      <c r="G5" s="3">
+        <v>43731</v>
+      </c>
+      <c r="H5" s="3">
+        <v>65874</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="3">
-        <v>29961</v>
-      </c>
-      <c r="C5" s="3">
-        <v>29162</v>
-      </c>
-      <c r="D5" s="3">
-        <v>43731</v>
-      </c>
-      <c r="E5" s="3">
-        <v>65874</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="3">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" s="3">
+        <v>435</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3">
+        <v>414</v>
+      </c>
+      <c r="F7" s="3">
+        <v>399</v>
+      </c>
+      <c r="G7" s="3">
+        <v>399</v>
+      </c>
+      <c r="H7" s="3">
+        <v>399</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="3">
-        <v>414</v>
-      </c>
-      <c r="C7" s="3">
-        <v>399</v>
-      </c>
-      <c r="D7" s="3">
-        <v>399</v>
-      </c>
-      <c r="E7" s="3">
-        <v>399</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2190</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>86</v>
+      </c>
+      <c r="G9" s="3">
+        <v>105</v>
+      </c>
+      <c r="H9" s="3">
+        <v>127</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="3">
-        <v>0</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3">
-        <v>86</v>
-      </c>
-      <c r="D9" s="3">
-        <v>105</v>
-      </c>
-      <c r="E9" s="3">
-        <v>127</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="B10" s="3">
-        <f t="shared" ref="B10" si="0">SUM(B3:B9)</f>
+        <f t="shared" ref="B10:E10" si="0">SUM(B3:B9)</f>
+        <v>307800</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
         <v>338192</v>
       </c>
-      <c r="C10" s="3">
-        <f t="shared" ref="C10:G10" si="1">SUM(C3:C9)</f>
+      <c r="F10" s="3">
+        <f t="shared" ref="F10:J10" si="1">SUM(F3:F9)</f>
         <v>343242</v>
       </c>
-      <c r="D10" s="3">
+      <c r="G10" s="3">
         <f t="shared" si="1"/>
         <v>353012</v>
       </c>
-      <c r="E10" s="3">
+      <c r="H10" s="3">
         <f t="shared" si="1"/>
         <v>358809</v>
       </c>
-      <c r="F10" s="3">
+      <c r="I10" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G10" s="3">
+      <c r="J10" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
-      <c r="C11" s="5">
-        <f>C10/B10-1</f>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5">
+        <f>F10/E10-1</f>
         <v>1.4932346122912499E-2</v>
       </c>
-      <c r="D11" s="5">
-        <f t="shared" ref="D11:E11" si="2">D10/C10-1</f>
+      <c r="G11" s="5">
+        <f t="shared" ref="G11:H11" si="2">G10/F10-1</f>
         <v>2.8463882625086701E-2</v>
       </c>
-      <c r="E11" s="5">
+      <c r="H11" s="5">
         <f t="shared" si="2"/>
         <v>1.642153807802571E-2</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
@@ -3025,183 +3092,236 @@
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="3">
+        <v>8411</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3">
+        <v>8770</v>
+      </c>
+      <c r="F13" s="3">
+        <v>8351</v>
+      </c>
+      <c r="G13" s="3">
+        <v>7960</v>
+      </c>
+      <c r="H13" s="3">
+        <v>7835</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="3">
-        <v>8770</v>
-      </c>
-      <c r="C13" s="3">
-        <v>8351</v>
-      </c>
-      <c r="D13" s="3">
-        <v>7960</v>
-      </c>
-      <c r="E13" s="3">
-        <v>7835</v>
-      </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
       <c r="B14" s="3">
+        <v>347</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3">
         <v>99</v>
       </c>
-      <c r="C14" s="3">
+      <c r="F14" s="3">
         <v>86</v>
       </c>
-      <c r="D14" s="3">
+      <c r="G14" s="3">
         <v>74</v>
       </c>
-      <c r="E14" s="3">
+      <c r="H14" s="3">
         <v>597</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="3">
+        <v>739</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3">
+        <v>423</v>
+      </c>
+      <c r="F15" s="3">
+        <v>421</v>
+      </c>
+      <c r="G15" s="3">
+        <v>420</v>
+      </c>
+      <c r="H15" s="3">
+        <v>418</v>
+      </c>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="3">
-        <v>423</v>
-      </c>
-      <c r="C15" s="3">
-        <v>421</v>
-      </c>
-      <c r="D15" s="3">
-        <v>420</v>
-      </c>
-      <c r="E15" s="3">
-        <v>418</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>66</v>
-      </c>
       <c r="B16" s="3">
-        <v>3422</v>
-      </c>
-      <c r="C16" s="3">
-        <v>3422</v>
-      </c>
-      <c r="D16" s="3">
-        <v>3422</v>
-      </c>
+        <v>2190</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
       <c r="E16" s="3">
         <v>3422</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F16" s="3">
+        <v>3422</v>
+      </c>
+      <c r="G16" s="3">
+        <v>3422</v>
+      </c>
+      <c r="H16" s="3">
+        <v>3422</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="3">
-        <f t="shared" ref="B17" si="3">SUM(B13:B16)</f>
+        <f t="shared" ref="B17:E17" si="3">SUM(B13:B16)</f>
+        <v>11687</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="3"/>
         <v>12714</v>
       </c>
-      <c r="C17" s="3">
-        <f t="shared" ref="C17:G17" si="4">SUM(C13:C16)</f>
+      <c r="F17" s="3">
+        <f t="shared" ref="F17:J17" si="4">SUM(F13:F16)</f>
         <v>12280</v>
       </c>
-      <c r="D17" s="3">
+      <c r="G17" s="3">
         <f t="shared" si="4"/>
         <v>11876</v>
       </c>
-      <c r="E17" s="3">
+      <c r="H17" s="3">
         <f t="shared" si="4"/>
         <v>12272</v>
       </c>
-      <c r="F17" s="3">
+      <c r="I17" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G17" s="3">
+      <c r="J17" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
-      <c r="C18" s="5">
-        <f>C17/B17-1</f>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5">
+        <f>F17/E17-1</f>
         <v>-3.413559855277648E-2</v>
       </c>
-      <c r="D18" s="5">
-        <f t="shared" ref="D18:E18" si="5">D17/C17-1</f>
+      <c r="G18" s="5">
+        <f t="shared" ref="G18:H18" si="5">G17/F17-1</f>
         <v>-3.2899022801302968E-2</v>
       </c>
-      <c r="E18" s="5">
+      <c r="H18" s="5">
         <f t="shared" si="5"/>
         <v>3.3344560458066663E-2</v>
       </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="3">
-        <f t="shared" ref="B19:G19" si="6">B10+B17</f>
-        <v>350906</v>
+        <f t="shared" ref="B19:E19" si="6">B10+B17</f>
+        <v>319487</v>
       </c>
       <c r="C19" s="3">
         <f t="shared" si="6"/>
-        <v>355522</v>
+        <v>0</v>
       </c>
       <c r="D19" s="3">
         <f t="shared" si="6"/>
-        <v>364888</v>
+        <v>0</v>
       </c>
       <c r="E19" s="3">
         <f t="shared" si="6"/>
+        <v>350906</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" ref="F19:J19" si="7">F10+F17</f>
+        <v>355522</v>
+      </c>
+      <c r="G19" s="3">
+        <f t="shared" si="7"/>
+        <v>364888</v>
+      </c>
+      <c r="H19" s="3">
+        <f t="shared" si="7"/>
         <v>371081</v>
       </c>
-      <c r="F19" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="3">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I19" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
-      <c r="C20" s="5">
-        <f>C19/B19-1</f>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5">
+        <f>F19/E19-1</f>
         <v>1.3154520013906934E-2</v>
       </c>
-      <c r="D20" s="5">
-        <f t="shared" ref="D20:E20" si="7">D19/C19-1</f>
+      <c r="G20" s="5">
+        <f t="shared" ref="G20:H20" si="8">G19/F19-1</f>
         <v>2.6344361249092785E-2</v>
       </c>
-      <c r="E20" s="5">
-        <f t="shared" si="7"/>
+      <c r="H20" s="5">
+        <f t="shared" si="8"/>
         <v>1.697233123588604E-2</v>
       </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
@@ -3209,205 +3329,263 @@
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="3">
+        <v>8334</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3">
+        <v>7950</v>
+      </c>
+      <c r="F22" s="3">
+        <v>7728</v>
+      </c>
+      <c r="G22" s="3">
+        <v>7503</v>
+      </c>
+      <c r="H22" s="3">
+        <v>7273</v>
+      </c>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="3">
-        <v>7950</v>
-      </c>
-      <c r="C22" s="3">
-        <v>7728</v>
-      </c>
-      <c r="D22" s="3">
-        <v>7503</v>
-      </c>
-      <c r="E22" s="3">
-        <v>7273</v>
-      </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B23" s="3">
+        <v>213</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3">
+        <v>394</v>
+      </c>
+      <c r="F23" s="3">
+        <v>312</v>
+      </c>
+      <c r="G23" s="3">
+        <v>229</v>
+      </c>
+      <c r="H23" s="3">
+        <v>144</v>
+      </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="3">
-        <v>394</v>
-      </c>
-      <c r="C23" s="3">
-        <v>312</v>
-      </c>
-      <c r="D23" s="3">
-        <v>229</v>
-      </c>
-      <c r="E23" s="3">
-        <v>144</v>
-      </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B24" s="3">
+        <v>7837</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3">
+        <v>2472</v>
+      </c>
+      <c r="F24" s="3">
+        <v>3206</v>
+      </c>
+      <c r="G24" s="3">
+        <v>3548</v>
+      </c>
+      <c r="H24" s="3">
+        <v>3534</v>
+      </c>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="3">
+        <v>88</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3">
+        <v>80</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0</v>
+      </c>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="3">
+        <v>4304</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3">
+        <v>4311</v>
+      </c>
+      <c r="F26" s="3">
+        <v>5787</v>
+      </c>
+      <c r="G26" s="3">
+        <v>9152</v>
+      </c>
+      <c r="H26" s="3">
+        <v>7065</v>
+      </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="3">
+        <v>973</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3">
+        <v>2109</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3">
+        <v>944</v>
+      </c>
+      <c r="H27" s="3">
+        <v>2272</v>
+      </c>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>70</v>
-      </c>
-      <c r="B24" s="3">
-        <v>2472</v>
-      </c>
-      <c r="C24" s="3">
-        <v>3206</v>
-      </c>
-      <c r="D24" s="3">
-        <v>3548</v>
-      </c>
-      <c r="E24" s="3">
-        <v>3534</v>
-      </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="3">
-        <v>80</v>
-      </c>
-      <c r="C25" s="3">
-        <v>0</v>
-      </c>
-      <c r="D25" s="3">
-        <v>0</v>
-      </c>
-      <c r="E25" s="3">
-        <v>0</v>
-      </c>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>67</v>
-      </c>
-      <c r="B26" s="3">
-        <v>4311</v>
-      </c>
-      <c r="C26" s="3">
-        <v>5787</v>
-      </c>
-      <c r="D26" s="3">
-        <v>9152</v>
-      </c>
-      <c r="E26" s="3">
-        <v>7065</v>
-      </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>80</v>
-      </c>
-      <c r="B27" s="3">
-        <v>2109</v>
-      </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3">
-        <v>944</v>
-      </c>
-      <c r="E27" s="3">
-        <v>2272</v>
-      </c>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>71</v>
       </c>
       <c r="B28" s="3">
         <v>213</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3">
         <v>213</v>
       </c>
-      <c r="D28" s="3">
+      <c r="F28" s="3">
         <v>213</v>
       </c>
-      <c r="E28" s="3">
+      <c r="G28" s="3">
+        <v>213</v>
+      </c>
+      <c r="H28" s="3">
         <v>330</v>
       </c>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3">
+        <v>0</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0</v>
+      </c>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+    </row>
+    <row r="30" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="3">
-        <v>0</v>
-      </c>
-      <c r="C29" s="3">
-        <v>0</v>
-      </c>
-      <c r="D29" s="3">
-        <v>0</v>
-      </c>
-      <c r="E29" s="3">
-        <v>0</v>
-      </c>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-    </row>
-    <row r="30" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="B30" s="3">
-        <f t="shared" ref="B30:E30" si="8">SUM(B22:B29)</f>
+        <f t="shared" ref="B30:E30" si="9">SUM(B22:B29)</f>
+        <v>21962</v>
+      </c>
+      <c r="C30" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="E30" s="3">
+        <f t="shared" si="9"/>
         <v>17529</v>
       </c>
-      <c r="C30" s="3">
-        <f t="shared" si="8"/>
+      <c r="F30" s="3">
+        <f t="shared" ref="F30:H30" si="10">SUM(F22:F29)</f>
         <v>17246</v>
       </c>
-      <c r="D30" s="3">
-        <f t="shared" si="8"/>
+      <c r="G30" s="3">
+        <f t="shared" si="10"/>
         <v>21589</v>
       </c>
-      <c r="E30" s="3">
-        <f t="shared" si="8"/>
+      <c r="H30" s="3">
+        <f t="shared" si="10"/>
         <v>20618</v>
       </c>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
-      <c r="C31" s="5">
-        <f>C30/B30-1</f>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5">
+        <f>F30/E30-1</f>
         <v>-1.6144674539334769E-2</v>
       </c>
-      <c r="D31" s="5">
-        <f t="shared" ref="D31:E31" si="9">D30/C30-1</f>
+      <c r="G31" s="5">
+        <f t="shared" ref="G31:H31" si="11">G30/F30-1</f>
         <v>0.25182651049518734</v>
       </c>
-      <c r="E31" s="5">
-        <f t="shared" si="9"/>
+      <c r="H31" s="5">
+        <f t="shared" si="11"/>
         <v>-4.4976608458010991E-2</v>
       </c>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
@@ -3415,112 +3593,145 @@
       <c r="M31" s="6"/>
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="3">
+        <v>0</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3">
+        <v>0</v>
+      </c>
+      <c r="G33" s="3">
+        <v>0</v>
+      </c>
+      <c r="H33" s="3">
+        <v>0</v>
+      </c>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="3">
-        <v>0</v>
-      </c>
-      <c r="C33" s="3">
-        <v>0</v>
-      </c>
-      <c r="D33" s="3">
-        <v>0</v>
-      </c>
-      <c r="E33" s="3">
-        <v>0</v>
-      </c>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B34" s="3">
+        <v>0</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3">
+        <v>0</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0</v>
+      </c>
+      <c r="G34" s="3">
+        <v>0</v>
+      </c>
+      <c r="H34" s="3">
+        <v>0</v>
+      </c>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="3">
-        <v>0</v>
-      </c>
-      <c r="C34" s="3">
-        <v>0</v>
-      </c>
-      <c r="D34" s="3">
-        <v>0</v>
-      </c>
-      <c r="E34" s="3">
-        <v>0</v>
-      </c>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>31</v>
-      </c>
       <c r="B35" s="3">
-        <v>6556</v>
-      </c>
-      <c r="C35" s="3">
-        <v>6556</v>
-      </c>
-      <c r="D35" s="3">
-        <v>6556</v>
-      </c>
+        <v>6495</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
       <c r="E35" s="3">
         <v>6556</v>
       </c>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-    </row>
-    <row r="36" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F35" s="3">
+        <v>6556</v>
+      </c>
+      <c r="G35" s="3">
+        <v>6556</v>
+      </c>
+      <c r="H35" s="3">
+        <v>6556</v>
+      </c>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B36" s="3">
-        <f t="shared" ref="B36:E36" si="10">SUM(B33:B35)</f>
+        <f t="shared" ref="B36:E36" si="12">SUM(B33:B35)</f>
+        <v>6495</v>
+      </c>
+      <c r="C36" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="D36" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="E36" s="3">
+        <f t="shared" si="12"/>
         <v>6556</v>
       </c>
-      <c r="C36" s="3">
-        <f t="shared" si="10"/>
+      <c r="F36" s="3">
+        <f t="shared" ref="F36:H36" si="13">SUM(F33:F35)</f>
         <v>6556</v>
       </c>
-      <c r="D36" s="3">
-        <f t="shared" si="10"/>
+      <c r="G36" s="3">
+        <f t="shared" si="13"/>
         <v>6556</v>
       </c>
-      <c r="E36" s="3">
-        <f t="shared" si="10"/>
+      <c r="H36" s="3">
+        <f t="shared" si="13"/>
         <v>6556</v>
       </c>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B37" s="5"/>
-      <c r="C37" s="5">
-        <f>C36/B36-1</f>
-        <v>0</v>
-      </c>
-      <c r="D37" s="5">
-        <f t="shared" ref="D37:E37" si="11">D36/C36-1</f>
-        <v>0</v>
-      </c>
-      <c r="E37" s="5">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5">
+        <f>F36/E36-1</f>
+        <v>0</v>
+      </c>
+      <c r="G37" s="5">
+        <f t="shared" ref="G37:H37" si="14">G36/F36-1</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="5">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
       <c r="K37" s="6"/>
@@ -3528,98 +3739,134 @@
       <c r="M37" s="6"/>
       <c r="N37" s="6"/>
       <c r="O37" s="6"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P37" s="6"/>
+      <c r="Q37" s="6"/>
+      <c r="R37" s="6"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-    </row>
-    <row r="39" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+    </row>
+    <row r="39" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B39" s="3">
-        <f t="shared" ref="B39:G39" si="12">B36+B30</f>
+        <f t="shared" ref="B39:E39" si="15">B36+B30</f>
+        <v>28457</v>
+      </c>
+      <c r="C39" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="D39" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="E39" s="3">
+        <f t="shared" si="15"/>
         <v>24085</v>
       </c>
-      <c r="C39" s="3">
-        <f t="shared" si="12"/>
+      <c r="F39" s="3">
+        <f t="shared" ref="F39:J39" si="16">F36+F30</f>
         <v>23802</v>
       </c>
-      <c r="D39" s="3">
-        <f t="shared" si="12"/>
+      <c r="G39" s="3">
+        <f t="shared" si="16"/>
         <v>28145</v>
       </c>
-      <c r="E39" s="3">
-        <f t="shared" si="12"/>
+      <c r="H39" s="3">
+        <f t="shared" si="16"/>
         <v>27174</v>
       </c>
-      <c r="F39" s="3">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="G39" s="3">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I39" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J39" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
-    </row>
-    <row r="41" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+    </row>
+    <row r="41" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="3">
+        <f t="shared" ref="B41:E41" si="17">B19-B39-B40</f>
+        <v>291030</v>
+      </c>
+      <c r="C41" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="D41" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="E41" s="3">
+        <f t="shared" si="17"/>
+        <v>326821</v>
+      </c>
+      <c r="F41" s="3">
+        <f>F19-F39-F40</f>
+        <v>331720</v>
+      </c>
+      <c r="G41" s="3">
+        <f>G19-G39-G40</f>
+        <v>336743</v>
+      </c>
+      <c r="H41" s="3">
+        <f>H19-H39-H40</f>
+        <v>343907</v>
+      </c>
+      <c r="I41" s="3">
+        <f>I19-I39</f>
+        <v>0</v>
+      </c>
+      <c r="J41" s="3">
+        <f>J19-J39</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="5">
+        <f>F41/E41-1</f>
+        <v>1.4989856832945181E-2</v>
+      </c>
+      <c r="G42" s="5">
+        <f t="shared" ref="G42" si="18">G41/F41-1</f>
+        <v>1.5142288677197691E-2</v>
+      </c>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>34</v>
-      </c>
-      <c r="B41" s="3">
-        <f>B19-B39-B40</f>
-        <v>326821</v>
-      </c>
-      <c r="C41" s="3">
-        <f>C19-C39-C40</f>
-        <v>331720</v>
-      </c>
-      <c r="D41" s="3">
-        <f>D19-D39-D40</f>
-        <v>336743</v>
-      </c>
-      <c r="E41" s="3">
-        <f>E19-E39-E40</f>
-        <v>343907</v>
-      </c>
-      <c r="F41" s="3">
-        <f>F19-F39</f>
-        <v>0</v>
-      </c>
-      <c r="G41" s="3">
-        <f>G19-G39</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="7"/>
-      <c r="C42" s="5">
-        <f>C41/B41-1</f>
-        <v>1.4989856832945181E-2</v>
-      </c>
-      <c r="D42" s="5">
-        <f t="shared" ref="D42" si="13">D41/C41-1</f>
-        <v>1.5142288677197691E-2</v>
-      </c>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>35</v>
       </c>
       <c r="B43" s="8">
         <v>800000000</v>
@@ -3633,419 +3880,571 @@
       <c r="E43" s="8">
         <v>800000000</v>
       </c>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F43" s="8">
+        <v>800000000</v>
+      </c>
+      <c r="G43" s="8">
+        <v>800000000</v>
+      </c>
+      <c r="H43" s="8">
+        <v>800000000</v>
+      </c>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="8">
+        <v>360</v>
+      </c>
+      <c r="C44" s="8">
+        <v>348</v>
+      </c>
+      <c r="D44" s="8">
+        <v>330</v>
+      </c>
+      <c r="E44" s="8">
+        <v>416</v>
+      </c>
+      <c r="F44" s="8">
+        <v>308</v>
+      </c>
+      <c r="G44" s="8">
+        <v>424</v>
+      </c>
+      <c r="H44" s="8">
+        <v>428</v>
+      </c>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>36</v>
       </c>
-      <c r="B44" s="8">
-        <v>416</v>
-      </c>
-      <c r="C44" s="8">
-        <v>308</v>
-      </c>
-      <c r="D44" s="8">
-        <v>424</v>
-      </c>
-      <c r="E44" s="8">
-        <v>428</v>
-      </c>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="B45" s="8">
+        <f t="shared" ref="B45:H45" si="19">B43*B44/1000000</f>
+        <v>288000</v>
+      </c>
+      <c r="C45" s="8">
+        <f t="shared" si="19"/>
+        <v>278400</v>
+      </c>
+      <c r="D45" s="8">
+        <f t="shared" si="19"/>
+        <v>264000</v>
+      </c>
+      <c r="E45" s="8">
+        <f t="shared" si="19"/>
+        <v>332800</v>
+      </c>
+      <c r="F45" s="8">
+        <f t="shared" si="19"/>
+        <v>246400</v>
+      </c>
+      <c r="G45" s="8">
+        <f t="shared" si="19"/>
+        <v>339200</v>
+      </c>
+      <c r="H45" s="8">
+        <f t="shared" si="19"/>
+        <v>342400</v>
+      </c>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>37</v>
       </c>
-      <c r="B45" s="8">
-        <f>B43*B44/1000000</f>
-        <v>332800</v>
-      </c>
-      <c r="C45" s="8">
-        <f>C43*C44/1000000</f>
-        <v>246400</v>
-      </c>
-      <c r="D45" s="8">
-        <f t="shared" ref="D45" si="14">D43*D44/1000000</f>
-        <v>339200</v>
-      </c>
-      <c r="E45" s="8">
-        <f>E43*E44/1000000</f>
-        <v>342400</v>
-      </c>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>38</v>
-      </c>
       <c r="B46" s="8">
-        <f t="shared" ref="B46:E46" si="15">B45+B22+B23+B24+B26+B28-B3-B7</f>
+        <f t="shared" ref="B46:H46" si="20">B45+B22+B23+B24+B26+B28-B3-B7</f>
+        <v>293930</v>
+      </c>
+      <c r="C46" s="8">
+        <f t="shared" si="20"/>
+        <v>278400</v>
+      </c>
+      <c r="D46" s="8">
+        <f t="shared" si="20"/>
+        <v>264000</v>
+      </c>
+      <c r="E46" s="8">
+        <f t="shared" si="20"/>
         <v>220422</v>
       </c>
-      <c r="C46" s="8">
-        <f t="shared" si="15"/>
+      <c r="F46" s="8">
+        <f t="shared" si="20"/>
         <v>146823</v>
       </c>
-      <c r="D46" s="8">
-        <f t="shared" si="15"/>
+      <c r="G46" s="8">
+        <f t="shared" si="20"/>
         <v>273349</v>
       </c>
-      <c r="E46" s="8">
-        <f t="shared" si="15"/>
+      <c r="H46" s="8">
+        <f t="shared" si="20"/>
         <v>286769</v>
       </c>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-    </row>
-    <row r="48" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+    </row>
+    <row r="48" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48" s="3">
+        <v>12370</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3">
+        <v>13194</v>
+      </c>
+      <c r="F48" s="3">
+        <v>10147</v>
+      </c>
+      <c r="G48" s="3">
+        <v>22097</v>
+      </c>
+      <c r="H48" s="3">
+        <v>35718</v>
+      </c>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B49" s="3">
+        <v>0</v>
+      </c>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3">
+        <v>0</v>
+      </c>
+      <c r="F49" s="3">
+        <v>0</v>
+      </c>
+      <c r="G49" s="3">
+        <v>0</v>
+      </c>
+      <c r="H49" s="3">
+        <v>0</v>
+      </c>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B50" s="3">
+        <f t="shared" ref="B50:E50" si="21">B48+B49</f>
+        <v>12370</v>
+      </c>
+      <c r="C50" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="D50" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="E50" s="3">
+        <f t="shared" si="21"/>
         <v>13194</v>
       </c>
-      <c r="C48" s="3">
+      <c r="F50" s="3">
+        <f t="shared" ref="F50:J50" si="22">F48+F49</f>
         <v>10147</v>
       </c>
-      <c r="D48" s="3">
+      <c r="G50" s="3">
+        <f t="shared" si="22"/>
         <v>22097</v>
       </c>
-      <c r="E48" s="3">
+      <c r="H50" s="3">
+        <f t="shared" si="22"/>
         <v>35718</v>
       </c>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B49" s="3">
-        <v>0</v>
-      </c>
-      <c r="C49" s="3">
-        <v>0</v>
-      </c>
-      <c r="D49" s="3">
-        <v>0</v>
-      </c>
-      <c r="E49" s="3">
-        <v>0</v>
-      </c>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
+      <c r="I50" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="J50" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>41</v>
       </c>
-      <c r="B50" s="3">
-        <f t="shared" ref="B50:G50" si="16">B48+B49</f>
-        <v>13194</v>
-      </c>
-      <c r="C50" s="3">
-        <f t="shared" si="16"/>
-        <v>10147</v>
-      </c>
-      <c r="D50" s="3">
-        <f t="shared" si="16"/>
-        <v>22097</v>
-      </c>
-      <c r="E50" s="3">
-        <f t="shared" si="16"/>
-        <v>35718</v>
-      </c>
-      <c r="F50" s="3">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="G50" s="3">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="B51" s="3">
+        <v>0</v>
+      </c>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3">
+        <v>0</v>
+      </c>
+      <c r="F51" s="3">
+        <v>0</v>
+      </c>
+      <c r="G51" s="3">
+        <v>0</v>
+      </c>
+      <c r="H51" s="3">
+        <v>0</v>
+      </c>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>42</v>
       </c>
-      <c r="B51" s="3">
-        <v>0</v>
-      </c>
-      <c r="C51" s="3">
-        <v>0</v>
-      </c>
-      <c r="D51" s="3">
-        <v>0</v>
-      </c>
-      <c r="E51" s="3">
-        <v>0</v>
-      </c>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="B52" s="3">
+        <v>-4587</v>
+      </c>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3">
+        <v>-4264</v>
+      </c>
+      <c r="F52" s="3">
+        <v>-4465</v>
+      </c>
+      <c r="G52" s="3">
+        <v>-9855</v>
+      </c>
+      <c r="H52" s="3">
+        <v>-14379</v>
+      </c>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53" s="3">
+        <v>-1472</v>
+      </c>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3">
+        <v>0</v>
+      </c>
+      <c r="F53" s="3">
+        <v>0</v>
+      </c>
+      <c r="G53" s="3">
+        <v>0</v>
+      </c>
+      <c r="H53" s="3">
+        <v>0</v>
+      </c>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>43</v>
       </c>
-      <c r="B52" s="3">
-        <v>-4264</v>
-      </c>
-      <c r="C52" s="3">
-        <v>-4465</v>
-      </c>
-      <c r="D52" s="3">
-        <v>-9855</v>
-      </c>
-      <c r="E52" s="3">
-        <v>-14379</v>
-      </c>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="B54" s="3">
+        <v>-173</v>
+      </c>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3">
+        <v>-171</v>
+      </c>
+      <c r="F54" s="3">
+        <v>-134</v>
+      </c>
+      <c r="G54" s="3">
+        <v>-260</v>
+      </c>
+      <c r="H54" s="3">
+        <v>-376</v>
+      </c>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>44</v>
       </c>
-      <c r="B53" s="3">
-        <v>-171</v>
-      </c>
-      <c r="C53" s="3">
-        <v>-134</v>
-      </c>
-      <c r="D53" s="3">
-        <v>-260</v>
-      </c>
-      <c r="E53" s="3">
-        <v>-376</v>
-      </c>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="B55" s="3">
+        <f t="shared" ref="B55:H55" si="23">SUM(B50:B54)</f>
+        <v>6138</v>
+      </c>
+      <c r="C55" s="3">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="D55" s="3">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="E55" s="3">
+        <f t="shared" si="23"/>
+        <v>8759</v>
+      </c>
+      <c r="F55" s="3">
+        <f t="shared" si="23"/>
+        <v>5548</v>
+      </c>
+      <c r="G55" s="3">
+        <f t="shared" si="23"/>
+        <v>11982</v>
+      </c>
+      <c r="H55" s="3">
+        <f t="shared" si="23"/>
+        <v>20963</v>
+      </c>
+      <c r="I55" s="3">
+        <f t="shared" ref="E55:J55" si="24">I50+I51+I52+I54</f>
+        <v>0</v>
+      </c>
+      <c r="J55" s="3">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>45</v>
       </c>
-      <c r="B54" s="3">
-        <f t="shared" ref="B54:G54" si="17">B50+B51+B52+B53</f>
-        <v>8759</v>
-      </c>
-      <c r="C54" s="3">
-        <f t="shared" si="17"/>
-        <v>5548</v>
-      </c>
-      <c r="D54" s="3">
-        <f t="shared" si="17"/>
-        <v>11982</v>
-      </c>
-      <c r="E54" s="3">
-        <f t="shared" si="17"/>
-        <v>20963</v>
-      </c>
-      <c r="F54" s="3">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="G54" s="3">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="B56" s="3">
+        <v>-1888</v>
+      </c>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3">
+        <v>-1740</v>
+      </c>
+      <c r="F56" s="3">
+        <v>-902</v>
+      </c>
+      <c r="G56" s="3">
+        <v>-2090</v>
+      </c>
+      <c r="H56" s="3">
+        <v>-3905</v>
+      </c>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>46</v>
       </c>
-      <c r="B55" s="3">
-        <v>-1740</v>
-      </c>
-      <c r="C55" s="3">
-        <v>-902</v>
-      </c>
-      <c r="D55" s="3">
-        <v>-2090</v>
-      </c>
-      <c r="E55" s="3">
-        <v>-3905</v>
-      </c>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="B57" s="3">
+        <f t="shared" ref="B57:H57" si="25">SUM(B55:B56)</f>
+        <v>4250</v>
+      </c>
+      <c r="C57" s="3">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="D57" s="3">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="E57" s="3">
+        <f t="shared" si="25"/>
+        <v>7019</v>
+      </c>
+      <c r="F57" s="3">
+        <f t="shared" si="25"/>
+        <v>4646</v>
+      </c>
+      <c r="G57" s="3">
+        <f t="shared" si="25"/>
+        <v>9892</v>
+      </c>
+      <c r="H57" s="3">
+        <f t="shared" si="25"/>
+        <v>17058</v>
+      </c>
+      <c r="I57" s="3">
+        <f t="shared" ref="E57:J57" si="26">I55+I56</f>
+        <v>0</v>
+      </c>
+      <c r="J57" s="3">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>47</v>
       </c>
-      <c r="B56" s="3">
-        <f t="shared" ref="B56:G56" si="18">B54+B55</f>
-        <v>7019</v>
-      </c>
-      <c r="C56" s="3">
-        <f t="shared" si="18"/>
-        <v>4646</v>
-      </c>
-      <c r="D56" s="3">
-        <f t="shared" si="18"/>
-        <v>9892</v>
-      </c>
-      <c r="E56" s="3">
-        <f t="shared" si="18"/>
-        <v>17058</v>
-      </c>
-      <c r="F56" s="3">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="G56" s="3">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>48</v>
-      </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5">
-        <f>C56/B56-1</f>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5">
+        <f t="shared" ref="B58:H58" si="27">C57/B57-1</f>
+        <v>-1</v>
+      </c>
+      <c r="D58" s="5" t="e">
+        <f t="shared" si="27"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E58" s="5" t="e">
+        <f t="shared" si="27"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F58" s="5">
+        <f t="shared" si="27"/>
         <v>-0.33808234791280811</v>
       </c>
-      <c r="D57" s="5">
-        <f t="shared" ref="D57:E57" si="19">D56/C56-1</f>
+      <c r="G58" s="5">
+        <f t="shared" si="27"/>
         <v>1.1291433491175202</v>
       </c>
-      <c r="E57" s="5">
-        <f t="shared" si="19"/>
+      <c r="H58" s="5">
+        <f t="shared" si="27"/>
         <v>0.72442377678932468</v>
       </c>
-      <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
-      <c r="H57" s="6"/>
-      <c r="I57" s="6"/>
-      <c r="J57" s="6"/>
-      <c r="K57" s="6"/>
-      <c r="L57" s="6"/>
-      <c r="M57" s="6"/>
-      <c r="N57" s="6"/>
-      <c r="O57" s="6"/>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5"/>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>49</v>
-      </c>
-      <c r="B59" s="7">
-        <f>(B56/B48)*(B48/B19)*(B19/B41)</f>
-        <v>2.1476588101743771E-2</v>
-      </c>
-      <c r="C59" s="7">
-        <f>(C56/C48)*(C48/C19)*(C19/C41)</f>
-        <v>1.4005788013987698E-2</v>
-      </c>
-      <c r="D59" s="7">
-        <f>(D56/D48)*(D48/D19)*(D19/D41)</f>
-        <v>2.9375517828135998E-2</v>
-      </c>
-      <c r="E59" s="7">
-        <f>(E56/E48)*(E48/E19)*(E19/E41)</f>
-        <v>4.9600618771935438E-2</v>
-      </c>
+      <c r="I58" s="6"/>
+      <c r="J58" s="6"/>
+      <c r="K58" s="6"/>
+      <c r="L58" s="6"/>
+      <c r="M58" s="6"/>
+      <c r="N58" s="6"/>
+      <c r="O58" s="6"/>
+      <c r="P58" s="6"/>
+      <c r="Q58" s="6"/>
+      <c r="R58" s="6"/>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>48</v>
+      </c>
+      <c r="B60" s="7">
+        <f t="shared" ref="B60:E63" si="28">(B57/B48)*(B48/B19)*(B19/B41)</f>
+        <v>1.4603305501151086E-2</v>
+      </c>
+      <c r="C60" s="7" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D60" s="7" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E60" s="7">
+        <f t="shared" si="28"/>
+        <v>2.1476588101743771E-2</v>
+      </c>
+      <c r="F60" s="7">
+        <f>(F57/F48)*(F48/F19)*(F19/F41)</f>
+        <v>1.4005788013987698E-2</v>
+      </c>
+      <c r="G60" s="7">
+        <f>(G57/G48)*(G48/G19)*(G19/G41)</f>
+        <v>2.9375517828135998E-2</v>
+      </c>
+      <c r="H60" s="7">
+        <f>(H57/H48)*(H48/H19)*(H19/H41)</f>
+        <v>4.9600618771935438E-2</v>
+      </c>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>49</v>
+      </c>
+      <c r="B61" s="7" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C61" s="7" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D61" s="7" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E61" s="7" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F61" s="7">
+        <f>F57/F48</f>
+        <v>0.4578693209815709</v>
+      </c>
+      <c r="G61" s="7">
+        <f>G57/G48</f>
+        <v>0.44766257863058334</v>
+      </c>
+      <c r="H61" s="7">
+        <f>H57/H48</f>
+        <v>0.47757433226944396</v>
+      </c>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>50</v>
       </c>
-      <c r="B60" s="7">
-        <f>B56/B48</f>
-        <v>0.53198423525845084</v>
-      </c>
-      <c r="C60" s="7">
-        <f>C56/C48</f>
-        <v>0.4578693209815709</v>
-      </c>
-      <c r="D60" s="7">
-        <f>D56/D48</f>
-        <v>0.44766257863058334</v>
-      </c>
-      <c r="E60" s="7">
-        <f>E56/E48</f>
-        <v>0.47757433226944396</v>
-      </c>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>51</v>
-      </c>
-      <c r="B61" s="5">
-        <f>ABS(B51/B48)</f>
-        <v>0</v>
-      </c>
-      <c r="C61" s="5">
-        <f>ABS(C51/C48)</f>
-        <v>0</v>
-      </c>
-      <c r="D61" s="5">
-        <f>ABS(D51/D48)</f>
-        <v>0</v>
-      </c>
-      <c r="E61" s="5">
-        <f>ABS(E51/E48)</f>
-        <v>0</v>
-      </c>
-      <c r="F61" s="6"/>
-      <c r="G61" s="6"/>
-      <c r="H61" s="6"/>
-      <c r="I61" s="6"/>
-      <c r="J61" s="6"/>
-      <c r="K61" s="6"/>
-      <c r="L61" s="6"/>
-      <c r="M61" s="6"/>
-      <c r="N61" s="6"/>
-      <c r="O61" s="6"/>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>52</v>
-      </c>
-      <c r="B62" s="7">
-        <f>ABS(B52/B48)</f>
-        <v>0.323177201758375</v>
-      </c>
-      <c r="C62" s="7">
-        <f>ABS(C52/C48)</f>
-        <v>0.44003153641470383</v>
-      </c>
-      <c r="D62" s="7">
-        <f>ABS(D52/D48)</f>
-        <v>0.44598814318685792</v>
-      </c>
-      <c r="E62" s="7">
-        <f>ABS(E52/E48)</f>
-        <v>0.40257013270619857</v>
-      </c>
-      <c r="F62" s="6"/>
-      <c r="G62" s="6"/>
-      <c r="H62" s="6"/>
+      <c r="B62" s="5" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C62" s="5" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D62" s="5" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E62" s="5" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F62" s="5">
+        <f>ABS(F51/F48)</f>
+        <v>0</v>
+      </c>
+      <c r="G62" s="5">
+        <f>ABS(G51/G48)</f>
+        <v>0</v>
+      </c>
+      <c r="H62" s="5">
+        <f>ABS(H51/H48)</f>
+        <v>0</v>
+      </c>
       <c r="I62" s="6"/>
       <c r="J62" s="6"/>
       <c r="K62" s="6"/>
@@ -4053,536 +4452,619 @@
       <c r="M62" s="6"/>
       <c r="N62" s="6"/>
       <c r="O62" s="6"/>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="P62" s="6"/>
+      <c r="Q62" s="6"/>
+      <c r="R62" s="6"/>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>51</v>
+      </c>
+      <c r="B63" s="7" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C63" s="7" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D63" s="7" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E63" s="7" t="e">
+        <f t="shared" si="28"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F63" s="7">
+        <f>ABS(F52/F48)</f>
+        <v>0.44003153641470383</v>
+      </c>
+      <c r="G63" s="7">
+        <f>ABS(G52/G48)</f>
+        <v>0.44598814318685792</v>
+      </c>
+      <c r="H63" s="7">
+        <f>ABS(H52/H48)</f>
+        <v>0.40257013270619857</v>
+      </c>
+      <c r="I63" s="6"/>
+      <c r="J63" s="6"/>
+      <c r="K63" s="6"/>
+      <c r="L63" s="6"/>
+      <c r="M63" s="6"/>
+      <c r="N63" s="6"/>
+      <c r="O63" s="6"/>
+      <c r="P63" s="6"/>
+      <c r="Q63" s="6"/>
+      <c r="R63" s="6"/>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
+      <c r="J64" s="3"/>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>72</v>
+      </c>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3">
+        <v>175524</v>
+      </c>
+      <c r="F65" s="3">
+        <v>187025</v>
+      </c>
+      <c r="G65" s="3">
+        <v>413878</v>
+      </c>
+      <c r="H65" s="3">
+        <v>702365</v>
+      </c>
+      <c r="I65" s="3">
+        <v>0</v>
+      </c>
+      <c r="J65" s="3">
+        <f t="shared" ref="J65:R65" si="29">I65*(1+J66)</f>
+        <v>0</v>
+      </c>
+      <c r="K65" s="10">
+        <v>0</v>
+      </c>
+      <c r="L65" s="10">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="M65" s="10">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="N65" s="10">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="O65" s="10">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="P65" s="10">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="Q65" s="10">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="R65" s="10">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="5">
+        <f t="shared" ref="F66:H66" si="30">F65/E65-1</f>
+        <v>6.5523803012693449E-2</v>
+      </c>
+      <c r="G66" s="5">
+        <f t="shared" si="30"/>
+        <v>1.2129554872343271</v>
+      </c>
+      <c r="H66" s="5">
+        <f t="shared" si="30"/>
+        <v>0.69703390854309721</v>
+      </c>
+      <c r="I66" s="6"/>
+      <c r="J66" s="6"/>
+      <c r="K66" s="6"/>
+      <c r="L66" s="6"/>
+      <c r="M66" s="6"/>
+      <c r="N66" s="6"/>
+      <c r="O66" s="6"/>
+      <c r="P66" s="6"/>
+      <c r="Q66" s="6"/>
+      <c r="R66" s="6"/>
+      <c r="S66" s="6"/>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>71</v>
+      </c>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3">
+        <v>115</v>
+      </c>
+      <c r="F67" s="3">
+        <v>115</v>
+      </c>
+      <c r="G67" s="3">
+        <v>175</v>
+      </c>
+      <c r="H67" s="3">
+        <v>270</v>
+      </c>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="10"/>
+      <c r="L67" s="10"/>
+      <c r="M67" s="10"/>
+      <c r="N67" s="10"/>
+      <c r="O67" s="10"/>
+      <c r="P67" s="10"/>
+      <c r="Q67" s="10"/>
+      <c r="R67" s="10"/>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="5">
+        <f>ABS(F67/F$65)</f>
+        <v>6.1489105734527469E-4</v>
+      </c>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="6"/>
+      <c r="J68" s="6"/>
+      <c r="K68" s="6"/>
+      <c r="L68" s="6"/>
+      <c r="M68" s="6"/>
+      <c r="N68" s="6"/>
+      <c r="O68" s="6"/>
+      <c r="P68" s="6"/>
+      <c r="Q68" s="6"/>
+      <c r="R68" s="6"/>
+      <c r="S68" s="6"/>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>73</v>
       </c>
-      <c r="B64" s="3">
-        <v>175524</v>
-      </c>
-      <c r="C64" s="3">
-        <v>187025</v>
-      </c>
-      <c r="D64" s="3">
-        <v>413878</v>
-      </c>
-      <c r="E64" s="3">
-        <v>702365</v>
-      </c>
-      <c r="F64" s="3">
-        <v>0</v>
-      </c>
-      <c r="G64" s="3">
-        <f t="shared" ref="G64:O64" si="20">F64*(1+G65)</f>
-        <v>0</v>
-      </c>
-      <c r="H64" s="10">
-        <v>0</v>
-      </c>
-      <c r="I64" s="10">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="J64" s="10">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="K64" s="10">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="L64" s="10">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="M64" s="10">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="N64" s="10">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="O64" s="10">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B65" s="3"/>
-      <c r="C65" s="5">
-        <f t="shared" ref="C65:E65" si="21">C64/B64-1</f>
-        <v>6.5523803012693449E-2</v>
-      </c>
-      <c r="D65" s="5">
-        <f t="shared" si="21"/>
-        <v>1.2129554872343271</v>
-      </c>
-      <c r="E65" s="5">
-        <f t="shared" si="21"/>
-        <v>0.69703390854309721</v>
-      </c>
-      <c r="F65" s="6"/>
-      <c r="G65" s="6"/>
-      <c r="H65" s="6"/>
-      <c r="I65" s="6"/>
-      <c r="J65" s="6"/>
-      <c r="K65" s="6"/>
-      <c r="L65" s="6"/>
-      <c r="M65" s="6"/>
-      <c r="N65" s="6"/>
-      <c r="O65" s="6"/>
-      <c r="P65" s="6"/>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>72</v>
-      </c>
-      <c r="B66" s="3">
-        <v>115</v>
-      </c>
-      <c r="C66" s="3">
-        <v>115</v>
-      </c>
-      <c r="D66" s="3">
-        <v>175</v>
-      </c>
-      <c r="E66" s="3">
-        <v>270</v>
-      </c>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
-      <c r="H66" s="10"/>
-      <c r="I66" s="10"/>
-      <c r="J66" s="10"/>
-      <c r="K66" s="10"/>
-      <c r="L66" s="10"/>
-      <c r="M66" s="10"/>
-      <c r="N66" s="10"/>
-      <c r="O66" s="10"/>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B67" s="3"/>
-      <c r="C67" s="5">
-        <f>ABS(C66/C$64)</f>
-        <v>6.1489105734527469E-4</v>
-      </c>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="6"/>
-      <c r="G67" s="6"/>
-      <c r="H67" s="6"/>
-      <c r="I67" s="6"/>
-      <c r="J67" s="6"/>
-      <c r="K67" s="6"/>
-      <c r="L67" s="6"/>
-      <c r="M67" s="6"/>
-      <c r="N67" s="6"/>
-      <c r="O67" s="6"/>
-      <c r="P67" s="6"/>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3">
+        <v>-106302</v>
+      </c>
+      <c r="F69" s="3">
+        <v>-192117</v>
+      </c>
+      <c r="G69" s="3">
+        <v>-441831</v>
+      </c>
+      <c r="H69" s="3">
+        <v>-737268</v>
+      </c>
+      <c r="I69" s="3"/>
+      <c r="J69" s="3"/>
+      <c r="K69" s="10"/>
+      <c r="L69" s="10"/>
+      <c r="M69" s="10"/>
+      <c r="N69" s="10"/>
+      <c r="O69" s="10"/>
+      <c r="P69" s="10"/>
+      <c r="Q69" s="10"/>
+      <c r="R69" s="10"/>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="5">
+        <f t="shared" ref="F70:H70" si="31">ABS(F69/F$65)</f>
+        <v>1.0272263066434968</v>
+      </c>
+      <c r="G70" s="5">
+        <f t="shared" si="31"/>
+        <v>1.0675392265353558</v>
+      </c>
+      <c r="H70" s="5">
+        <f t="shared" si="31"/>
+        <v>1.0496935354124992</v>
+      </c>
+      <c r="I70" s="6"/>
+      <c r="J70" s="6"/>
+      <c r="K70" s="6"/>
+      <c r="L70" s="6"/>
+      <c r="M70" s="6"/>
+      <c r="N70" s="6"/>
+      <c r="O70" s="6"/>
+      <c r="P70" s="6"/>
+      <c r="Q70" s="6"/>
+      <c r="R70" s="6"/>
+      <c r="S70" s="6"/>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>74</v>
       </c>
-      <c r="B68" s="3">
-        <v>-106302</v>
-      </c>
-      <c r="C68" s="3">
-        <v>-192117</v>
-      </c>
-      <c r="D68" s="3">
-        <v>-441831</v>
-      </c>
-      <c r="E68" s="3">
-        <v>-737268</v>
-      </c>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
-      <c r="H68" s="10"/>
-      <c r="I68" s="10"/>
-      <c r="J68" s="10"/>
-      <c r="K68" s="10"/>
-      <c r="L68" s="10"/>
-      <c r="M68" s="10"/>
-      <c r="N68" s="10"/>
-      <c r="O68" s="10"/>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B69" s="3"/>
-      <c r="C69" s="5">
-        <f t="shared" ref="C69:E69" si="22">ABS(C68/C$64)</f>
-        <v>1.0272263066434968</v>
-      </c>
-      <c r="D69" s="5">
-        <f t="shared" si="22"/>
-        <v>1.0675392265353558</v>
-      </c>
-      <c r="E69" s="5">
-        <f t="shared" si="22"/>
-        <v>1.0496935354124992</v>
-      </c>
-      <c r="F69" s="6"/>
-      <c r="G69" s="6"/>
-      <c r="H69" s="6"/>
-      <c r="I69" s="6"/>
-      <c r="J69" s="6"/>
-      <c r="K69" s="6"/>
-      <c r="L69" s="6"/>
-      <c r="M69" s="6"/>
-      <c r="N69" s="6"/>
-      <c r="O69" s="6"/>
-      <c r="P69" s="6"/>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3">
+        <v>-171</v>
+      </c>
+      <c r="F71" s="3">
+        <v>-134</v>
+      </c>
+      <c r="G71" s="3">
+        <v>-260</v>
+      </c>
+      <c r="H71" s="3">
+        <v>-376</v>
+      </c>
+      <c r="I71" s="3"/>
+      <c r="J71" s="3"/>
+      <c r="K71" s="10"/>
+      <c r="L71" s="10"/>
+      <c r="M71" s="10"/>
+      <c r="N71" s="10"/>
+      <c r="O71" s="10"/>
+      <c r="P71" s="10"/>
+      <c r="Q71" s="10"/>
+      <c r="R71" s="10"/>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="5">
+        <f t="shared" ref="F72:H72" si="32">ABS(F71/F$65)</f>
+        <v>7.164817537762331E-4</v>
+      </c>
+      <c r="G72" s="5">
+        <f t="shared" si="32"/>
+        <v>6.2820444672101439E-4</v>
+      </c>
+      <c r="H72" s="5">
+        <f t="shared" si="32"/>
+        <v>5.3533419233589368E-4</v>
+      </c>
+      <c r="I72" s="6"/>
+      <c r="J72" s="6"/>
+      <c r="K72" s="6"/>
+      <c r="L72" s="6"/>
+      <c r="M72" s="6"/>
+      <c r="N72" s="6"/>
+      <c r="O72" s="6"/>
+      <c r="P72" s="6"/>
+      <c r="Q72" s="6"/>
+      <c r="R72" s="6"/>
+      <c r="S72" s="6"/>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>75</v>
       </c>
-      <c r="B70" s="3">
-        <v>-171</v>
-      </c>
-      <c r="C70" s="3">
-        <v>-134</v>
-      </c>
-      <c r="D70" s="3">
-        <v>-260</v>
-      </c>
-      <c r="E70" s="3">
-        <v>-376</v>
-      </c>
-      <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
-      <c r="H70" s="10"/>
-      <c r="I70" s="10"/>
-      <c r="J70" s="10"/>
-      <c r="K70" s="10"/>
-      <c r="L70" s="10"/>
-      <c r="M70" s="10"/>
-      <c r="N70" s="10"/>
-      <c r="O70" s="10"/>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B71" s="3"/>
-      <c r="C71" s="5">
-        <f t="shared" ref="C71:E71" si="23">ABS(C70/C$64)</f>
-        <v>7.164817537762331E-4</v>
-      </c>
-      <c r="D71" s="5">
-        <f t="shared" si="23"/>
-        <v>6.2820444672101439E-4</v>
-      </c>
-      <c r="E71" s="5">
-        <f t="shared" si="23"/>
-        <v>5.3533419233589368E-4</v>
-      </c>
-      <c r="F71" s="6"/>
-      <c r="G71" s="6"/>
-      <c r="H71" s="6"/>
-      <c r="I71" s="6"/>
-      <c r="J71" s="6"/>
-      <c r="K71" s="6"/>
-      <c r="L71" s="6"/>
-      <c r="M71" s="6"/>
-      <c r="N71" s="6"/>
-      <c r="O71" s="6"/>
-      <c r="P71" s="6"/>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3">
+        <v>-3794</v>
+      </c>
+      <c r="F73" s="3">
+        <v>-2251</v>
+      </c>
+      <c r="G73" s="3">
+        <v>-8471</v>
+      </c>
+      <c r="H73" s="3">
+        <v>-11885</v>
+      </c>
+      <c r="I73" s="3"/>
+      <c r="J73" s="3"/>
+      <c r="K73" s="3"/>
+      <c r="L73" s="3"/>
+      <c r="M73" s="3"/>
+      <c r="N73" s="3"/>
+      <c r="O73" s="3"/>
+      <c r="P73" s="3"/>
+      <c r="Q73" s="3"/>
+      <c r="R73" s="3"/>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="7">
+        <f t="shared" ref="F74:H74" si="33">ABS(F73/F$65)</f>
+        <v>1.2035824087688812E-2</v>
+      </c>
+      <c r="G74" s="7">
+        <f t="shared" si="33"/>
+        <v>2.0467384108360433E-2</v>
+      </c>
+      <c r="H74" s="7">
+        <f t="shared" si="33"/>
+        <v>1.6921401265723661E-2</v>
+      </c>
+      <c r="I74" s="6"/>
+      <c r="J74" s="6"/>
+      <c r="K74" s="6"/>
+      <c r="L74" s="6"/>
+      <c r="M74" s="6"/>
+      <c r="N74" s="6"/>
+      <c r="O74" s="6"/>
+      <c r="P74" s="6"/>
+      <c r="Q74" s="6"/>
+      <c r="R74" s="6"/>
+      <c r="S74" s="6"/>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>76</v>
       </c>
-      <c r="B72" s="3">
-        <v>-3794</v>
-      </c>
-      <c r="C72" s="3">
-        <v>-2251</v>
-      </c>
-      <c r="D72" s="3">
-        <v>-8471</v>
-      </c>
-      <c r="E72" s="3">
-        <v>-11885</v>
-      </c>
-      <c r="F72" s="3"/>
-      <c r="G72" s="3"/>
-      <c r="H72" s="3"/>
-      <c r="I72" s="3"/>
-      <c r="J72" s="3"/>
-      <c r="K72" s="3"/>
-      <c r="L72" s="3"/>
-      <c r="M72" s="3"/>
-      <c r="N72" s="3"/>
-      <c r="O72" s="3"/>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B73" s="3"/>
-      <c r="C73" s="7">
-        <f t="shared" ref="C73:E73" si="24">ABS(C72/C$64)</f>
-        <v>1.2035824087688812E-2</v>
-      </c>
-      <c r="D73" s="7">
-        <f t="shared" si="24"/>
-        <v>2.0467384108360433E-2</v>
-      </c>
-      <c r="E73" s="7">
-        <f t="shared" si="24"/>
-        <v>1.6921401265723661E-2</v>
-      </c>
-      <c r="F73" s="6"/>
-      <c r="G73" s="6"/>
-      <c r="H73" s="6"/>
-      <c r="I73" s="6"/>
-      <c r="J73" s="6"/>
-      <c r="K73" s="6"/>
-      <c r="L73" s="6"/>
-      <c r="M73" s="6"/>
-      <c r="N73" s="6"/>
-      <c r="O73" s="6"/>
-      <c r="P73" s="6"/>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3">
+        <v>0</v>
+      </c>
+      <c r="F75" s="3">
+        <v>-396</v>
+      </c>
+      <c r="G75" s="3">
+        <v>-792</v>
+      </c>
+      <c r="H75" s="3">
+        <v>-1188</v>
+      </c>
+      <c r="I75" s="3"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="3"/>
+      <c r="L75" s="3"/>
+      <c r="M75" s="3"/>
+      <c r="N75" s="3"/>
+      <c r="O75" s="3"/>
+      <c r="P75" s="3"/>
+      <c r="Q75" s="3"/>
+      <c r="R75" s="3"/>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="7">
+        <f t="shared" ref="F76:H76" si="34">ABS(F75/F$65)</f>
+        <v>2.1173639887715548E-3</v>
+      </c>
+      <c r="G76" s="7">
+        <f t="shared" si="34"/>
+        <v>1.913607391550167E-3</v>
+      </c>
+      <c r="H76" s="7">
+        <f t="shared" si="34"/>
+        <v>1.6914282459974514E-3</v>
+      </c>
+      <c r="I76" s="6"/>
+      <c r="J76" s="6"/>
+      <c r="K76" s="6"/>
+      <c r="L76" s="6"/>
+      <c r="M76" s="6"/>
+      <c r="N76" s="6"/>
+      <c r="O76" s="6"/>
+      <c r="P76" s="6"/>
+      <c r="Q76" s="6"/>
+      <c r="R76" s="6"/>
+      <c r="S76" s="6"/>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>77</v>
       </c>
-      <c r="B74" s="3">
-        <v>0</v>
-      </c>
-      <c r="C74" s="3">
-        <v>-396</v>
-      </c>
-      <c r="D74" s="3">
-        <v>-792</v>
-      </c>
-      <c r="E74" s="3">
-        <v>-1188</v>
-      </c>
-      <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
-      <c r="H74" s="3"/>
-      <c r="I74" s="3"/>
-      <c r="J74" s="3"/>
-      <c r="K74" s="3"/>
-      <c r="L74" s="3"/>
-      <c r="M74" s="3"/>
-      <c r="N74" s="3"/>
-      <c r="O74" s="3"/>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B75" s="3"/>
-      <c r="C75" s="7">
-        <f t="shared" ref="C75:E75" si="25">ABS(C74/C$64)</f>
-        <v>2.1173639887715548E-3</v>
-      </c>
-      <c r="D75" s="7">
-        <f t="shared" si="25"/>
-        <v>1.913607391550167E-3</v>
-      </c>
-      <c r="E75" s="7">
-        <f t="shared" si="25"/>
-        <v>1.6914282459974514E-3</v>
-      </c>
-      <c r="F75" s="6"/>
-      <c r="G75" s="6"/>
-      <c r="H75" s="6"/>
-      <c r="I75" s="6"/>
-      <c r="J75" s="6"/>
-      <c r="K75" s="6"/>
-      <c r="L75" s="6"/>
-      <c r="M75" s="6"/>
-      <c r="N75" s="6"/>
-      <c r="O75" s="6"/>
-      <c r="P75" s="6"/>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>78</v>
-      </c>
-      <c r="B76" s="3">
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3">
         <v>-2881</v>
       </c>
-      <c r="C76" s="3">
+      <c r="F77" s="3">
         <v>-2816</v>
       </c>
-      <c r="D76" s="3">
+      <c r="G77" s="3">
         <v>-3277</v>
       </c>
-      <c r="E76" s="3">
+      <c r="H77" s="3">
         <v>-3807</v>
       </c>
-      <c r="F76" s="3"/>
-      <c r="G76" s="3"/>
-      <c r="H76" s="3"/>
-      <c r="I76" s="3"/>
-      <c r="J76" s="3"/>
-      <c r="K76" s="3"/>
-      <c r="L76" s="3"/>
-      <c r="M76" s="3"/>
-      <c r="N76" s="3"/>
-      <c r="O76" s="3"/>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B77" s="3"/>
-      <c r="C77" s="7">
-        <f t="shared" ref="C77:E77" si="26">ABS(C76/C$64)</f>
+      <c r="I77" s="3"/>
+      <c r="J77" s="3"/>
+      <c r="K77" s="3"/>
+      <c r="L77" s="3"/>
+      <c r="M77" s="3"/>
+      <c r="N77" s="3"/>
+      <c r="O77" s="3"/>
+      <c r="P77" s="3"/>
+      <c r="Q77" s="3"/>
+      <c r="R77" s="3"/>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="7">
+        <f t="shared" ref="F78:H78" si="35">ABS(F77/F$65)</f>
         <v>1.5056810586819944E-2</v>
       </c>
-      <c r="D77" s="7">
-        <f t="shared" si="26"/>
+      <c r="G78" s="7">
+        <f t="shared" si="35"/>
         <v>7.9177921996337088E-3</v>
       </c>
-      <c r="E77" s="7">
-        <f t="shared" si="26"/>
+      <c r="H78" s="7">
+        <f t="shared" si="35"/>
         <v>5.4202586974009242E-3</v>
       </c>
-      <c r="F77" s="11"/>
-      <c r="G77" s="11"/>
-      <c r="H77" s="11"/>
-      <c r="I77" s="11"/>
-      <c r="J77" s="11"/>
-      <c r="K77" s="11"/>
-      <c r="L77" s="11"/>
-      <c r="M77" s="11"/>
-      <c r="N77" s="11"/>
-      <c r="O77" s="11"/>
-      <c r="P77" s="6"/>
-    </row>
-    <row r="78" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B78" s="3">
-        <f t="shared" ref="B78:E78" si="27">B64+B66+B68+B70+B72+B74+B76</f>
+      <c r="I78" s="11"/>
+      <c r="J78" s="11"/>
+      <c r="K78" s="11"/>
+      <c r="L78" s="11"/>
+      <c r="M78" s="11"/>
+      <c r="N78" s="11"/>
+      <c r="O78" s="11"/>
+      <c r="P78" s="11"/>
+      <c r="Q78" s="11"/>
+      <c r="R78" s="11"/>
+      <c r="S78" s="6"/>
+    </row>
+    <row r="79" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3">
+        <f t="shared" ref="E79:H79" si="36">E65+E67+E69+E71+E73+E75+E77</f>
         <v>62491</v>
       </c>
-      <c r="C78" s="3">
-        <f t="shared" si="27"/>
+      <c r="F79" s="3">
+        <f t="shared" si="36"/>
         <v>-10574</v>
       </c>
-      <c r="D78" s="3">
-        <f t="shared" si="27"/>
+      <c r="G79" s="3">
+        <f t="shared" si="36"/>
         <v>-40578</v>
       </c>
-      <c r="E78" s="3">
-        <f t="shared" si="27"/>
+      <c r="H79" s="3">
+        <f t="shared" si="36"/>
         <v>-51889</v>
       </c>
-      <c r="F78" s="3"/>
-      <c r="G78" s="3"/>
-      <c r="H78" s="3"/>
-      <c r="I78" s="3"/>
-      <c r="J78" s="3"/>
-      <c r="K78" s="3"/>
-      <c r="L78" s="3"/>
-      <c r="M78" s="3"/>
-      <c r="N78" s="3"/>
-      <c r="O78" s="3"/>
-      <c r="P78" s="10"/>
-    </row>
-    <row r="79" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="4"/>
-      <c r="B79" s="3"/>
-      <c r="C79" s="5">
-        <f t="shared" ref="C79:E79" si="28">(C78/B78)-1</f>
-        <v>-1.1692083660047046</v>
-      </c>
-      <c r="D79" s="5">
-        <f t="shared" si="28"/>
-        <v>2.8375260071874409</v>
-      </c>
-      <c r="E79" s="5">
-        <f t="shared" si="28"/>
-        <v>0.27874710434225447</v>
-      </c>
-      <c r="F79" s="5"/>
-      <c r="G79" s="5"/>
-      <c r="H79" s="5"/>
-      <c r="I79" s="5"/>
-      <c r="J79" s="5"/>
-      <c r="K79" s="5"/>
-      <c r="L79" s="5"/>
-      <c r="M79" s="5"/>
-      <c r="N79" s="5"/>
-      <c r="O79" s="5"/>
-      <c r="P79" s="6"/>
-    </row>
-    <row r="80" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I79" s="3"/>
+      <c r="J79" s="3"/>
+      <c r="K79" s="3"/>
+      <c r="L79" s="3"/>
+      <c r="M79" s="3"/>
+      <c r="N79" s="3"/>
+      <c r="O79" s="3"/>
+      <c r="P79" s="3"/>
+      <c r="Q79" s="3"/>
+      <c r="R79" s="3"/>
+      <c r="S79" s="10"/>
+    </row>
+    <row r="80" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="3"/>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
-      <c r="E80" s="5"/>
-      <c r="F80" s="8"/>
-      <c r="G80" s="8"/>
-      <c r="H80" s="8"/>
-      <c r="I80" s="8"/>
-      <c r="J80" s="8"/>
-      <c r="K80" s="8"/>
-      <c r="L80" s="8"/>
-      <c r="M80" s="8"/>
-      <c r="N80" s="8"/>
-      <c r="O80" s="8"/>
-      <c r="P80" s="8"/>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>54</v>
-      </c>
-      <c r="B81" s="5"/>
-      <c r="C81" s="5"/>
-      <c r="D81" s="5"/>
-      <c r="E81" s="5"/>
-      <c r="F81" s="6"/>
-      <c r="G81" s="6"/>
-      <c r="H81" s="6"/>
-      <c r="I81" s="6"/>
-      <c r="J81" s="6"/>
-      <c r="K81" s="6"/>
-      <c r="L81" s="6"/>
-      <c r="M81" s="6"/>
-      <c r="N81" s="6"/>
-      <c r="O81" s="6"/>
-      <c r="P81" s="6"/>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="5">
+        <f t="shared" ref="F80:H80" si="37">(F79/E79)-1</f>
+        <v>-1.1692083660047046</v>
+      </c>
+      <c r="G80" s="5">
+        <f t="shared" si="37"/>
+        <v>2.8375260071874409</v>
+      </c>
+      <c r="H80" s="5">
+        <f t="shared" si="37"/>
+        <v>0.27874710434225447</v>
+      </c>
+      <c r="I80" s="5"/>
+      <c r="J80" s="5"/>
+      <c r="K80" s="5"/>
+      <c r="L80" s="5"/>
+      <c r="M80" s="5"/>
+      <c r="N80" s="5"/>
+      <c r="O80" s="5"/>
+      <c r="P80" s="5"/>
+      <c r="Q80" s="5"/>
+      <c r="R80" s="5"/>
+      <c r="S80" s="6"/>
+    </row>
+    <row r="81" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="4"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="5"/>
+      <c r="H81" s="5"/>
+      <c r="I81" s="8"/>
+      <c r="J81" s="8"/>
+      <c r="K81" s="8"/>
+      <c r="L81" s="8"/>
+      <c r="M81" s="8"/>
+      <c r="N81" s="8"/>
+      <c r="O81" s="8"/>
+      <c r="P81" s="8"/>
+      <c r="Q81" s="8"/>
+      <c r="R81" s="8"/>
+      <c r="S81" s="8"/>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>55</v>
-      </c>
-      <c r="B82" s="3"/>
+        <v>53</v>
+      </c>
+      <c r="B82" s="5"/>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="5"/>
-      <c r="F82" s="8"/>
-      <c r="G82" s="8"/>
-      <c r="H82" s="8"/>
-      <c r="I82" s="8"/>
-      <c r="J82" s="8"/>
-      <c r="K82" s="8"/>
-      <c r="L82" s="8"/>
-      <c r="M82" s="8"/>
-      <c r="N82" s="8"/>
-      <c r="O82" s="8"/>
-      <c r="P82" s="8"/>
-    </row>
-    <row r="83" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A83" s="4" t="s">
-        <v>56</v>
+      <c r="F82" s="5"/>
+      <c r="G82" s="5"/>
+      <c r="H82" s="5"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="6"/>
+      <c r="K82" s="6"/>
+      <c r="L82" s="6"/>
+      <c r="M82" s="6"/>
+      <c r="N82" s="6"/>
+      <c r="O82" s="6"/>
+      <c r="P82" s="6"/>
+      <c r="Q82" s="6"/>
+      <c r="R82" s="6"/>
+      <c r="S82" s="6"/>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>54</v>
       </c>
       <c r="B83" s="3"/>
-      <c r="C83" s="5"/>
-      <c r="D83" s="5"/>
-      <c r="E83" s="12"/>
-      <c r="F83" s="8"/>
-      <c r="G83" s="8"/>
-      <c r="H83" s="8"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="5"/>
+      <c r="G83" s="5"/>
+      <c r="H83" s="5"/>
       <c r="I83" s="8"/>
       <c r="J83" s="8"/>
       <c r="K83" s="8"/>
@@ -4591,18 +5073,21 @@
       <c r="N83" s="8"/>
       <c r="O83" s="8"/>
       <c r="P83" s="8"/>
-    </row>
-    <row r="84" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q83" s="8"/>
+      <c r="R83" s="8"/>
+      <c r="S83" s="8"/>
+    </row>
+    <row r="84" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B84" s="3"/>
-      <c r="C84" s="5"/>
-      <c r="D84" s="5"/>
-      <c r="E84" s="5"/>
-      <c r="F84" s="8"/>
-      <c r="G84" s="8"/>
-      <c r="H84" s="8"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
+      <c r="H84" s="12"/>
       <c r="I84" s="8"/>
       <c r="J84" s="8"/>
       <c r="K84" s="8"/>
@@ -4611,16 +5096,21 @@
       <c r="N84" s="8"/>
       <c r="O84" s="8"/>
       <c r="P84" s="8"/>
-    </row>
-    <row r="85" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A85" s="4"/>
+      <c r="Q84" s="8"/>
+      <c r="R84" s="8"/>
+      <c r="S84" s="8"/>
+    </row>
+    <row r="85" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="B85" s="3"/>
-      <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
-      <c r="E85" s="12"/>
-      <c r="F85" s="8"/>
-      <c r="G85" s="8"/>
-      <c r="H85" s="8"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="5"/>
+      <c r="H85" s="5"/>
       <c r="I85" s="8"/>
       <c r="J85" s="8"/>
       <c r="K85" s="8"/>
@@ -4629,316 +5119,375 @@
       <c r="N85" s="8"/>
       <c r="O85" s="8"/>
       <c r="P85" s="8"/>
-    </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q85" s="8"/>
+      <c r="R85" s="8"/>
+      <c r="S85" s="8"/>
+    </row>
+    <row r="86" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="4"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
       <c r="F86" s="5"/>
-      <c r="G86" s="3"/>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>58</v>
-      </c>
-      <c r="B87" s="3">
-        <v>-18</v>
-      </c>
-      <c r="C87" s="3">
-        <v>0</v>
-      </c>
-      <c r="D87" s="3">
-        <v>-15</v>
-      </c>
-      <c r="E87" s="3">
-        <v>-324</v>
-      </c>
+      <c r="G86" s="5"/>
+      <c r="H86" s="12"/>
+      <c r="I86" s="8"/>
+      <c r="J86" s="8"/>
+      <c r="K86" s="8"/>
+      <c r="L86" s="8"/>
+      <c r="M86" s="8"/>
+      <c r="N86" s="8"/>
+      <c r="O86" s="8"/>
+      <c r="P86" s="8"/>
+      <c r="Q86" s="8"/>
+      <c r="R86" s="8"/>
+      <c r="S86" s="8"/>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H87" s="3"/>
+      <c r="I87" s="5"/>
+      <c r="J87" s="3"/>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>81</v>
-      </c>
-      <c r="B88" s="3">
-        <v>0</v>
-      </c>
-      <c r="C88" s="3">
-        <v>0</v>
-      </c>
-      <c r="D88" s="3">
-        <v>0</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
       <c r="E88" s="3">
+        <v>-18</v>
+      </c>
+      <c r="F88" s="3">
+        <v>0</v>
+      </c>
+      <c r="G88" s="3">
+        <v>-15</v>
+      </c>
+      <c r="H88" s="3">
+        <v>-324</v>
+      </c>
+      <c r="I88" s="3"/>
+      <c r="J88" s="3"/>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>80</v>
+      </c>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3">
+        <v>0</v>
+      </c>
+      <c r="F89" s="3">
+        <v>0</v>
+      </c>
+      <c r="G89" s="3">
+        <v>0</v>
+      </c>
+      <c r="H89" s="3">
         <v>-584</v>
       </c>
-      <c r="F88" s="3"/>
-      <c r="G88" s="3"/>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="I89" s="3"/>
+      <c r="J89" s="3"/>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>58</v>
+      </c>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3">
+        <v>0</v>
+      </c>
+      <c r="F90" s="3">
+        <v>0</v>
+      </c>
+      <c r="G90" s="3">
+        <v>0</v>
+      </c>
+      <c r="H90" s="3">
+        <v>0</v>
+      </c>
+      <c r="I90" s="3"/>
+      <c r="J90" s="3"/>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>59</v>
       </c>
-      <c r="B89" s="3">
-        <v>0</v>
-      </c>
-      <c r="C89" s="3">
-        <v>0</v>
-      </c>
-      <c r="D89" s="3">
-        <v>0</v>
-      </c>
-      <c r="E89" s="3">
-        <v>0</v>
-      </c>
-      <c r="F89" s="3"/>
-      <c r="G89" s="3"/>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3">
+        <v>0</v>
+      </c>
+      <c r="F91" s="3">
+        <v>0</v>
+      </c>
+      <c r="G91" s="3">
+        <v>0</v>
+      </c>
+      <c r="H91" s="3">
+        <v>0</v>
+      </c>
+      <c r="I91" s="3"/>
+      <c r="J91" s="3"/>
+    </row>
+    <row r="92" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B90" s="3">
-        <v>0</v>
-      </c>
-      <c r="C90" s="3">
-        <v>0</v>
-      </c>
-      <c r="D90" s="3">
-        <v>0</v>
-      </c>
-      <c r="E90" s="3">
-        <v>0</v>
-      </c>
-      <c r="F90" s="3"/>
-      <c r="G90" s="3"/>
-    </row>
-    <row r="91" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="4" t="s">
+      <c r="B92" s="13"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="13"/>
+      <c r="E92" s="13">
+        <f t="shared" ref="E92:J92" si="38">SUM(E88:E91)</f>
+        <v>-18</v>
+      </c>
+      <c r="F92" s="13">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="G92" s="3">
+        <f t="shared" si="38"/>
+        <v>-15</v>
+      </c>
+      <c r="H92" s="3">
+        <f t="shared" si="38"/>
+        <v>-908</v>
+      </c>
+      <c r="I92" s="3">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="J92" s="3">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="5">
+        <f t="shared" ref="F93:H93" si="39">IFERROR(F92/E92-1,0)</f>
+        <v>-1</v>
+      </c>
+      <c r="G93" s="5">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="H93" s="5">
+        <f t="shared" si="39"/>
+        <v>59.533333333333331</v>
+      </c>
+      <c r="I93" s="6"/>
+      <c r="J93" s="6"/>
+      <c r="K93" s="6"/>
+      <c r="L93" s="6"/>
+      <c r="M93" s="6"/>
+      <c r="N93" s="6"/>
+      <c r="O93" s="6"/>
+      <c r="P93" s="6"/>
+      <c r="Q93" s="6"/>
+      <c r="R93" s="6"/>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>61</v>
       </c>
-      <c r="B91" s="13">
-        <f t="shared" ref="B91:G91" si="29">SUM(B87:B90)</f>
-        <v>-18</v>
-      </c>
-      <c r="C91" s="13">
-        <f t="shared" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="D91" s="3">
-        <f t="shared" si="29"/>
-        <v>-15</v>
-      </c>
-      <c r="E91" s="3">
-        <f t="shared" si="29"/>
-        <v>-908</v>
-      </c>
-      <c r="F91" s="3">
-        <f t="shared" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="G91" s="3">
-        <f t="shared" si="29"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B92" s="3"/>
-      <c r="C92" s="5">
-        <f t="shared" ref="C92:E92" si="30">IFERROR(C91/B91-1,0)</f>
-        <v>-1</v>
-      </c>
-      <c r="D92" s="5">
-        <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="E92" s="5">
-        <f t="shared" si="30"/>
-        <v>59.533333333333331</v>
-      </c>
-      <c r="F92" s="6"/>
-      <c r="G92" s="6"/>
-      <c r="H92" s="6"/>
-      <c r="I92" s="6"/>
-      <c r="J92" s="6"/>
-      <c r="K92" s="6"/>
-      <c r="L92" s="6"/>
-      <c r="M92" s="6"/>
-      <c r="N92" s="6"/>
-      <c r="O92" s="6"/>
-    </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="B94" s="3"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3">
+        <v>-301</v>
+      </c>
+      <c r="F94" s="3">
+        <v>-221</v>
+      </c>
+      <c r="G94" s="3">
+        <v>-446</v>
+      </c>
+      <c r="H94" s="3">
+        <v>-676</v>
+      </c>
+      <c r="I94" s="3"/>
+      <c r="J94" s="3"/>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>28</v>
+      </c>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3">
+        <v>0</v>
+      </c>
+      <c r="F95" s="3">
+        <v>0</v>
+      </c>
+      <c r="G95" s="3">
+        <v>0</v>
+      </c>
+      <c r="H95" s="3">
+        <v>0</v>
+      </c>
+      <c r="I95" s="3"/>
+      <c r="J95" s="3"/>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>78</v>
+      </c>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3">
+        <v>-81</v>
+      </c>
+      <c r="F96" s="3">
+        <v>-76</v>
+      </c>
+      <c r="G96" s="3">
+        <v>-165</v>
+      </c>
+      <c r="H96" s="3">
+        <v>-249</v>
+      </c>
+      <c r="I96" s="3"/>
+      <c r="J96" s="3"/>
+    </row>
+    <row r="97" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B93" s="3">
-        <v>-301</v>
-      </c>
-      <c r="C93" s="3">
-        <v>-221</v>
-      </c>
-      <c r="D93" s="3">
-        <v>-446</v>
-      </c>
-      <c r="E93" s="3">
-        <v>-676</v>
-      </c>
-      <c r="F93" s="3"/>
-      <c r="G93" s="3"/>
-    </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>29</v>
-      </c>
-      <c r="B94" s="3">
-        <v>0</v>
-      </c>
-      <c r="C94" s="3">
-        <v>0</v>
-      </c>
-      <c r="D94" s="3">
-        <v>0</v>
-      </c>
-      <c r="E94" s="3">
-        <v>0</v>
-      </c>
-      <c r="F94" s="3"/>
-      <c r="G94" s="3"/>
-    </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>79</v>
-      </c>
-      <c r="B95" s="3">
-        <v>-81</v>
-      </c>
-      <c r="C95" s="3">
-        <v>-76</v>
-      </c>
-      <c r="D95" s="3">
-        <v>-165</v>
-      </c>
-      <c r="E95" s="3">
-        <v>-249</v>
-      </c>
-      <c r="F95" s="3"/>
-      <c r="G95" s="3"/>
-    </row>
-    <row r="96" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A96" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B96" s="13">
-        <f>SUM(B93:B95)</f>
+      <c r="B97" s="13"/>
+      <c r="C97" s="13"/>
+      <c r="D97" s="13"/>
+      <c r="E97" s="13">
+        <f t="shared" ref="C97:J97" si="40">SUM(E94:E96)</f>
         <v>-382</v>
       </c>
-      <c r="C96" s="13">
-        <f>SUM(C93:C95)</f>
+      <c r="F97" s="13">
+        <f t="shared" si="40"/>
         <v>-297</v>
       </c>
-      <c r="D96" s="3">
-        <f>SUM(D93:D95)</f>
+      <c r="G97" s="3">
+        <f t="shared" si="40"/>
         <v>-611</v>
       </c>
-      <c r="E96" s="3">
-        <f>SUM(E93:E95)</f>
+      <c r="H97" s="3">
+        <f t="shared" si="40"/>
         <v>-925</v>
       </c>
-      <c r="F96" s="3">
-        <f>SUM(F93:F95)</f>
-        <v>0</v>
-      </c>
-      <c r="G96" s="3">
-        <f>SUM(G93:G95)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C97" s="5">
-        <f t="shared" ref="C97:E97" si="31">IFERROR(C96/B96-1,0)</f>
+      <c r="I97" s="3">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="J97" s="3">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F98" s="5">
+        <f t="shared" ref="F98:H98" si="41">IFERROR(F97/E97-1,0)</f>
         <v>-0.22251308900523559</v>
       </c>
-      <c r="D97" s="5">
-        <f t="shared" si="31"/>
+      <c r="G98" s="5">
+        <f t="shared" si="41"/>
         <v>1.0572390572390571</v>
       </c>
-      <c r="E97" s="5">
-        <f t="shared" si="31"/>
+      <c r="H98" s="5">
+        <f t="shared" si="41"/>
         <v>0.51391162029459903</v>
       </c>
-      <c r="F97" s="6"/>
-      <c r="G97" s="6"/>
-      <c r="H97" s="6"/>
-      <c r="I97" s="6"/>
-      <c r="J97" s="6"/>
-      <c r="K97" s="6"/>
-      <c r="L97" s="6"/>
-      <c r="M97" s="6"/>
-      <c r="N97" s="6"/>
-      <c r="O97" s="6"/>
-    </row>
-    <row r="98" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C98" s="3"/>
-    </row>
-    <row r="99" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C99" s="3"/>
-    </row>
-    <row r="100" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C100" s="3"/>
-    </row>
-    <row r="101" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C101" s="3"/>
-    </row>
-    <row r="102" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C102" s="3"/>
-    </row>
-    <row r="103" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C103" s="3"/>
-    </row>
-    <row r="104" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C104" s="3"/>
-    </row>
-    <row r="105" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C105" s="3"/>
-    </row>
-    <row r="106" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C106" s="3"/>
-    </row>
-    <row r="107" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C107" s="3"/>
-    </row>
-    <row r="108" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C108" s="3"/>
-    </row>
-    <row r="109" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C109" s="3"/>
-    </row>
-    <row r="110" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C110" s="3"/>
-    </row>
-    <row r="111" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C111" s="3"/>
-    </row>
-    <row r="112" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C112" s="3"/>
-    </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C113" s="3"/>
-    </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C114" s="3"/>
-    </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C115" s="3"/>
-    </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C116" s="3"/>
+      <c r="I98" s="6"/>
+      <c r="J98" s="6"/>
+      <c r="K98" s="6"/>
+      <c r="L98" s="6"/>
+      <c r="M98" s="6"/>
+      <c r="N98" s="6"/>
+      <c r="O98" s="6"/>
+      <c r="P98" s="6"/>
+      <c r="Q98" s="6"/>
+      <c r="R98" s="6"/>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F99" s="3"/>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F100" s="3"/>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F101" s="3"/>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F102" s="3"/>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F103" s="3"/>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F104" s="3"/>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F105" s="3"/>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F106" s="3"/>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F107" s="3"/>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F108" s="3"/>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F109" s="3"/>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F110" s="3"/>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F111" s="3"/>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F112" s="3"/>
+    </row>
+    <row r="113" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F113" s="3"/>
+    </row>
+    <row r="114" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F114" s="3"/>
+    </row>
+    <row r="115" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F115" s="3"/>
+    </row>
+    <row r="116" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F116" s="3"/>
+    </row>
+    <row r="117" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F117" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="C19:G19" formula="1"/>
+    <ignoredError sqref="F19:J19" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>